<commit_message>
0.0.14: Now generate toJSON Method.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002DDFF0-77D6-F346-B501-20020B826B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B177DC84-619B-404C-88D7-4CCF0C1DD994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
   <si>
     <t>クラス名</t>
   </si>
@@ -524,6 +524,13 @@
     </rPh>
     <rPh sb="27" eb="28">
       <t xml:space="preserve">ツカワレマス。 </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>toJSONから除外</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">ジョガイ </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -1734,10 +1741,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48:L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1747,33 +1754,33 @@
     <col min="8" max="8" width="9.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="28" style="1" customWidth="1"/>
-    <col min="15" max="15" width="33.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="11" max="12" width="9.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="28" style="1" customWidth="1"/>
+    <col min="16" max="16" width="33.33203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19">
+    <row r="1" spans="1:15" ht="19">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1787,8 +1794,9 @@
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
       <c r="K5" s="38"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="L5" s="38"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1804,9 +1812,10 @@
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
       <c r="K6" s="38"/>
-      <c r="L6" s="39"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="L6" s="38"/>
+      <c r="M6" s="39"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1822,9 +1831,10 @@
       <c r="I7" s="38"/>
       <c r="J7" s="38"/>
       <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="L7" s="38"/>
+      <c r="M7" s="39"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
         <v>84</v>
       </c>
@@ -1842,9 +1852,10 @@
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
       <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="L8" s="38"/>
+      <c r="M8" s="39"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1860,9 +1871,10 @@
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="L9" s="38"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="80" t="s">
         <v>74</v>
       </c>
@@ -1880,9 +1892,10 @@
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
       <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="L10" s="38"/>
+      <c r="M10" s="39"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -1900,9 +1913,10 @@
       <c r="I11" s="38"/>
       <c r="J11" s="38"/>
       <c r="K11" s="38"/>
-      <c r="L11" s="39"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="L11" s="38"/>
+      <c r="M11" s="39"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -1918,9 +1932,10 @@
       <c r="I12" s="38"/>
       <c r="J12" s="38"/>
       <c r="K12" s="38"/>
-      <c r="L12" s="39"/>
-    </row>
-    <row r="13" spans="1:14" ht="29" customHeight="1">
+      <c r="L12" s="38"/>
+      <c r="M12" s="39"/>
+    </row>
+    <row r="13" spans="1:15" ht="29" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1936,11 +1951,12 @@
       <c r="I13" s="69"/>
       <c r="J13" s="69"/>
       <c r="K13" s="69"/>
-      <c r="L13" s="38"/>
+      <c r="L13" s="69"/>
       <c r="M13" s="38"/>
       <c r="N13" s="38"/>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13" s="38"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -1959,8 +1975,9 @@
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
       <c r="N14" s="38"/>
-    </row>
-    <row r="15" spans="1:14" s="33" customFormat="1">
+      <c r="O14" s="38"/>
+    </row>
+    <row r="15" spans="1:15" s="33" customFormat="1">
       <c r="A15" s="66" t="s">
         <v>37</v>
       </c>
@@ -1974,9 +1991,10 @@
       <c r="I15" s="70"/>
       <c r="J15" s="70"/>
       <c r="K15" s="73"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:14" s="33" customFormat="1">
+      <c r="L15" s="73"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:15" s="33" customFormat="1">
       <c r="A16" s="66" t="s">
         <v>63</v>
       </c>
@@ -1994,9 +2012,10 @@
       <c r="I16" s="70"/>
       <c r="J16" s="70"/>
       <c r="K16" s="73"/>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:16" s="33" customFormat="1">
+      <c r="L16" s="73"/>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:17" s="33" customFormat="1">
       <c r="A17" s="66" t="s">
         <v>61</v>
       </c>
@@ -2010,9 +2029,10 @@
       <c r="I17" s="70"/>
       <c r="J17" s="70"/>
       <c r="K17" s="73"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:16" s="33" customFormat="1">
+      <c r="L17" s="73"/>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:17" s="33" customFormat="1">
       <c r="A18" s="92" t="s">
         <v>77</v>
       </c>
@@ -2028,9 +2048,10 @@
       <c r="I18" s="70"/>
       <c r="J18" s="70"/>
       <c r="K18" s="73"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:16" s="33" customFormat="1">
+      <c r="L18" s="73"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:17" s="33" customFormat="1">
       <c r="A19" s="66" t="s">
         <v>62</v>
       </c>
@@ -2046,9 +2067,10 @@
       <c r="I19" s="70"/>
       <c r="J19" s="70"/>
       <c r="K19" s="73"/>
-      <c r="L19"/>
-    </row>
-    <row r="20" spans="1:16" s="33" customFormat="1">
+      <c r="L19" s="73"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:17" s="33" customFormat="1">
       <c r="A20" s="66" t="s">
         <v>44</v>
       </c>
@@ -2064,9 +2086,10 @@
       <c r="I20" s="70"/>
       <c r="J20" s="70"/>
       <c r="K20" s="73"/>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:16" s="33" customFormat="1">
+      <c r="L20" s="73"/>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:17" s="33" customFormat="1">
       <c r="A21" s="66" t="s">
         <v>46</v>
       </c>
@@ -2082,9 +2105,10 @@
       <c r="I21" s="70"/>
       <c r="J21" s="70"/>
       <c r="K21" s="73"/>
-      <c r="L21"/>
-    </row>
-    <row r="22" spans="1:16" s="33" customFormat="1">
+      <c r="L21" s="73"/>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:17" s="33" customFormat="1">
       <c r="A22" s="92" t="s">
         <v>72</v>
       </c>
@@ -2102,9 +2126,10 @@
       <c r="I22" s="70"/>
       <c r="J22" s="70"/>
       <c r="K22" s="73"/>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:16" s="41" customFormat="1">
+      <c r="L22" s="73"/>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:17" s="41" customFormat="1">
       <c r="A23" s="38"/>
       <c r="B23" s="40"/>
       <c r="C23" s="38"/>
@@ -2119,8 +2144,9 @@
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="O23" s="38"/>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="31" t="s">
         <v>16</v>
       </c>
@@ -2135,12 +2161,13 @@
       <c r="J24" s="48"/>
       <c r="K24" s="48"/>
       <c r="L24" s="48"/>
-      <c r="M24" s="33"/>
+      <c r="M24" s="48"/>
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
       <c r="P24" s="33"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24" s="33"/>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="34" t="s">
         <v>0</v>
       </c>
@@ -2155,12 +2182,13 @@
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
       <c r="L25" s="71"/>
-      <c r="M25" s="33"/>
+      <c r="M25" s="71"/>
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="33"/>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
@@ -2174,9 +2202,10 @@
       <c r="I26" s="38"/>
       <c r="J26" s="38"/>
       <c r="K26" s="38"/>
-      <c r="L26" s="39"/>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="L26" s="38"/>
+      <c r="M26" s="39"/>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
@@ -2190,9 +2219,10 @@
       <c r="I27" s="38"/>
       <c r="J27" s="38"/>
       <c r="K27" s="38"/>
-      <c r="L27" s="39"/>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="L27" s="38"/>
+      <c r="M27" s="39"/>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="38"/>
       <c r="B28" s="40"/>
       <c r="C28" s="38"/>
@@ -2204,9 +2234,10 @@
       <c r="I28" s="38"/>
       <c r="J28" s="38"/>
       <c r="K28" s="38"/>
-      <c r="L28" s="39"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="L28" s="38"/>
+      <c r="M28" s="39"/>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="31" t="s">
         <v>56</v>
       </c>
@@ -2221,12 +2252,13 @@
       <c r="J29" s="48"/>
       <c r="K29" s="48"/>
       <c r="L29" s="48"/>
-      <c r="M29" s="47"/>
+      <c r="M29" s="48"/>
       <c r="N29" s="47"/>
       <c r="O29" s="47"/>
       <c r="P29" s="47"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="47"/>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="51" t="s">
         <v>32</v>
       </c>
@@ -2243,12 +2275,13 @@
       <c r="J30" s="71"/>
       <c r="K30" s="71"/>
       <c r="L30" s="71"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="49"/>
+      <c r="M30" s="71"/>
+      <c r="N30" s="48"/>
       <c r="O30" s="49"/>
-      <c r="P30" s="39"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="P30" s="49"/>
+      <c r="Q30" s="39"/>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="55"/>
       <c r="B31" s="50"/>
       <c r="C31" s="42"/>
@@ -2260,13 +2293,14 @@
       <c r="I31" s="72"/>
       <c r="J31" s="72"/>
       <c r="K31" s="72"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="40"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="38"/>
       <c r="N31" s="40"/>
       <c r="O31" s="40"/>
-      <c r="P31" s="39"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="P31" s="40"/>
+      <c r="Q31" s="39"/>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" s="55"/>
       <c r="B32" s="50"/>
       <c r="C32" s="44"/>
@@ -2278,13 +2312,14 @@
       <c r="I32" s="72"/>
       <c r="J32" s="72"/>
       <c r="K32" s="72"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="40"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="38"/>
       <c r="N32" s="40"/>
       <c r="O32" s="40"/>
-      <c r="P32" s="39"/>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="P32" s="40"/>
+      <c r="Q32" s="39"/>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="56"/>
       <c r="B33" s="52"/>
       <c r="C33" s="53"/>
@@ -2296,13 +2331,14 @@
       <c r="I33" s="72"/>
       <c r="J33" s="72"/>
       <c r="K33" s="72"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="40"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="38"/>
       <c r="N33" s="40"/>
       <c r="O33" s="40"/>
-      <c r="P33" s="39"/>
-    </row>
-    <row r="34" spans="1:16" s="41" customFormat="1">
+      <c r="P33" s="40"/>
+      <c r="Q33" s="39"/>
+    </row>
+    <row r="34" spans="1:17" s="41" customFormat="1">
       <c r="A34" s="38"/>
       <c r="B34" s="40"/>
       <c r="C34" s="38"/>
@@ -2317,8 +2353,9 @@
       <c r="L34" s="38"/>
       <c r="M34" s="38"/>
       <c r="N34" s="38"/>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="O34" s="38"/>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" s="31" t="s">
         <v>31</v>
       </c>
@@ -2333,12 +2370,13 @@
       <c r="J35" s="48"/>
       <c r="K35" s="48"/>
       <c r="L35" s="48"/>
-      <c r="M35" s="47"/>
+      <c r="M35" s="48"/>
       <c r="N35" s="47"/>
       <c r="O35" s="47"/>
       <c r="P35" s="47"/>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35" s="47"/>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36" s="51" t="s">
         <v>32</v>
       </c>
@@ -2355,12 +2393,13 @@
       <c r="J36" s="71"/>
       <c r="K36" s="71"/>
       <c r="L36" s="71"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="49"/>
+      <c r="M36" s="71"/>
+      <c r="N36" s="48"/>
       <c r="O36" s="49"/>
-      <c r="P36" s="39"/>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="P36" s="49"/>
+      <c r="Q36" s="39"/>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37" s="55">
         <v>1</v>
       </c>
@@ -2376,13 +2415,14 @@
       <c r="I37" s="72"/>
       <c r="J37" s="72"/>
       <c r="K37" s="72"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="40"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="38"/>
       <c r="N37" s="40"/>
       <c r="O37" s="40"/>
-      <c r="P37" s="39"/>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="P37" s="40"/>
+      <c r="Q37" s="39"/>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" s="55"/>
       <c r="B38" s="50"/>
       <c r="C38" s="44"/>
@@ -2394,13 +2434,14 @@
       <c r="I38" s="72"/>
       <c r="J38" s="72"/>
       <c r="K38" s="72"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="40"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="38"/>
       <c r="N38" s="40"/>
       <c r="O38" s="40"/>
-      <c r="P38" s="39"/>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="P38" s="40"/>
+      <c r="Q38" s="39"/>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" s="56"/>
       <c r="B39" s="52"/>
       <c r="C39" s="53"/>
@@ -2412,13 +2453,14 @@
       <c r="I39" s="72"/>
       <c r="J39" s="72"/>
       <c r="K39" s="72"/>
-      <c r="L39" s="38"/>
-      <c r="M39" s="40"/>
+      <c r="L39" s="72"/>
+      <c r="M39" s="38"/>
       <c r="N39" s="40"/>
       <c r="O39" s="40"/>
-      <c r="P39" s="39"/>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="P39" s="40"/>
+      <c r="Q39" s="39"/>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2432,8 +2474,9 @@
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="N40" s="13"/>
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41" s="31" t="s">
         <v>70</v>
       </c>
@@ -2448,12 +2491,13 @@
       <c r="J41" s="48"/>
       <c r="K41" s="48"/>
       <c r="L41" s="48"/>
-      <c r="M41" s="47"/>
+      <c r="M41" s="48"/>
       <c r="N41" s="47"/>
       <c r="O41" s="47"/>
       <c r="P41" s="47"/>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="Q41" s="47"/>
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42" s="51" t="s">
         <v>32</v>
       </c>
@@ -2470,12 +2514,13 @@
       <c r="J42" s="71"/>
       <c r="K42" s="71"/>
       <c r="L42" s="71"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="49"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="48"/>
       <c r="O42" s="49"/>
-      <c r="P42" s="39"/>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="P42" s="49"/>
+      <c r="Q42" s="39"/>
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43" s="55"/>
       <c r="B43" s="50"/>
       <c r="C43" s="42"/>
@@ -2487,13 +2532,14 @@
       <c r="I43" s="72"/>
       <c r="J43" s="72"/>
       <c r="K43" s="72"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="40"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="38"/>
       <c r="N43" s="40"/>
       <c r="O43" s="40"/>
-      <c r="P43" s="39"/>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="P43" s="40"/>
+      <c r="Q43" s="39"/>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44" s="55"/>
       <c r="B44" s="50"/>
       <c r="C44" s="44"/>
@@ -2505,13 +2551,14 @@
       <c r="I44" s="72"/>
       <c r="J44" s="72"/>
       <c r="K44" s="72"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="40"/>
+      <c r="L44" s="72"/>
+      <c r="M44" s="38"/>
       <c r="N44" s="40"/>
       <c r="O44" s="40"/>
-      <c r="P44" s="39"/>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="P44" s="40"/>
+      <c r="Q44" s="39"/>
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45" s="56"/>
       <c r="B45" s="52"/>
       <c r="C45" s="53"/>
@@ -2523,13 +2570,14 @@
       <c r="I45" s="72"/>
       <c r="J45" s="72"/>
       <c r="K45" s="72"/>
-      <c r="L45" s="38"/>
-      <c r="M45" s="40"/>
+      <c r="L45" s="72"/>
+      <c r="M45" s="38"/>
       <c r="N45" s="40"/>
       <c r="O45" s="40"/>
-      <c r="P45" s="39"/>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="P45" s="40"/>
+      <c r="Q45" s="39"/>
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -2543,8 +2591,9 @@
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
       <c r="M46" s="13"/>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="N46" s="13"/>
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47" s="3" t="s">
         <v>11</v>
       </c>
@@ -2561,10 +2610,11 @@
       <c r="L47" s="14"/>
       <c r="M47" s="14"/>
       <c r="N47" s="14"/>
-      <c r="O47" s="6"/>
-      <c r="P47" s="15"/>
-    </row>
-    <row r="48" spans="1:16" ht="13.5" customHeight="1">
+      <c r="O47" s="14"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="15"/>
+    </row>
+    <row r="48" spans="1:17" ht="13.5" customHeight="1">
       <c r="A48" s="86" t="s">
         <v>32</v>
       </c>
@@ -2598,15 +2648,18 @@
       <c r="K48" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="L48" s="85" t="s">
+      <c r="L48" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="M48" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="M48" s="85"/>
-      <c r="N48" s="16"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="9"/>
-    </row>
-    <row r="49" spans="1:16">
+      <c r="N48" s="85"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="9"/>
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49" s="86"/>
       <c r="B49" s="86"/>
       <c r="C49" s="85"/>
@@ -2618,13 +2671,14 @@
       <c r="I49" s="88"/>
       <c r="J49" s="91"/>
       <c r="K49" s="91"/>
-      <c r="L49" s="85"/>
+      <c r="L49" s="91"/>
       <c r="M49" s="85"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="30"/>
-      <c r="P49" s="15"/>
-    </row>
-    <row r="50" spans="1:16">
+      <c r="N49" s="85"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="30"/>
+      <c r="Q49" s="15"/>
+    </row>
+    <row r="50" spans="1:17">
       <c r="A50" s="19">
         <v>1</v>
       </c>
@@ -2650,15 +2704,16 @@
       <c r="K50" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="L50" s="21" t="s">
+      <c r="L50" s="78"/>
+      <c r="M50" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M50" s="22"/>
       <c r="N50" s="22"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="15"/>
-    </row>
-    <row r="51" spans="1:16">
+      <c r="O50" s="22"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="15"/>
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51" s="19">
         <f>A50+1</f>
         <v>2</v>
@@ -2683,13 +2738,14 @@
       <c r="K51" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="L51" s="21"/>
-      <c r="M51" s="22"/>
+      <c r="L51" s="78"/>
+      <c r="M51" s="21"/>
       <c r="N51" s="22"/>
-      <c r="O51" s="29"/>
-      <c r="P51" s="15"/>
-    </row>
-    <row r="52" spans="1:16">
+      <c r="O51" s="22"/>
+      <c r="P51" s="29"/>
+      <c r="Q51" s="15"/>
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52" s="19">
         <f t="shared" ref="A52:A54" si="0">A51+1</f>
         <v>3</v>
@@ -2712,15 +2768,16 @@
       </c>
       <c r="J52" s="78"/>
       <c r="K52" s="78"/>
-      <c r="L52" s="21" t="s">
+      <c r="L52" s="78"/>
+      <c r="M52" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M52" s="22"/>
       <c r="N52" s="22"/>
-      <c r="O52" s="23"/>
-      <c r="P52" s="15"/>
-    </row>
-    <row r="53" spans="1:16">
+      <c r="O52" s="22"/>
+      <c r="P52" s="23"/>
+      <c r="Q52" s="15"/>
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2743,15 +2800,18 @@
       <c r="I53" s="78"/>
       <c r="J53" s="78"/>
       <c r="K53" s="78"/>
-      <c r="L53" s="21" t="s">
+      <c r="L53" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="M53" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="M53" s="22"/>
       <c r="N53" s="22"/>
-      <c r="O53" s="23"/>
-      <c r="P53" s="15"/>
-    </row>
-    <row r="54" spans="1:16">
+      <c r="O53" s="22"/>
+      <c r="P53" s="23"/>
+      <c r="Q53" s="15"/>
+    </row>
+    <row r="54" spans="1:17">
       <c r="A54" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2774,15 +2834,16 @@
       <c r="I54" s="78"/>
       <c r="J54" s="78"/>
       <c r="K54" s="78"/>
-      <c r="L54" s="21" t="s">
+      <c r="L54" s="78"/>
+      <c r="M54" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="M54" s="22"/>
       <c r="N54" s="22"/>
-      <c r="O54" s="23"/>
-      <c r="P54" s="15"/>
-    </row>
-    <row r="55" spans="1:16">
+      <c r="O54" s="22"/>
+      <c r="P54" s="23"/>
+      <c r="Q54" s="15"/>
+    </row>
+    <row r="55" spans="1:17">
       <c r="A55" s="24"/>
       <c r="B55" s="25"/>
       <c r="C55" s="26"/>
@@ -2794,17 +2855,19 @@
       <c r="I55" s="79"/>
       <c r="J55" s="79"/>
       <c r="K55" s="79"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="27"/>
+      <c r="L55" s="79"/>
+      <c r="M55" s="26"/>
       <c r="N55" s="27"/>
-      <c r="O55" s="28"/>
-      <c r="P55" s="15"/>
+      <c r="O55" s="27"/>
+      <c r="P55" s="28"/>
+      <c r="Q55" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="K48:K49"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C13:G13"/>
-    <mergeCell ref="L48:M49"/>
+    <mergeCell ref="M48:N49"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="C48:C49"/>
@@ -2812,7 +2875,7 @@
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="I48:I49"/>
-    <mergeCell ref="K48:K49"/>
+    <mergeCell ref="L48:L49"/>
     <mergeCell ref="J48:J49"/>
     <mergeCell ref="H48:H49"/>
     <mergeCell ref="A22:B22"/>
@@ -2821,7 +2884,7 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G71:K71" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G71:L71" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2856,7 +2919,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I50:K55</xm:sqref>
+          <xm:sqref>I50:L55</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>